<commit_message>
midnight problem figured out
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E5D85-0CE0-CF44-AD57-B95B1F704336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D43ADBD-2478-154E-925B-7A76CFA64313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -31,26 +31,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Zoel</t>
-  </si>
-  <si>
-    <t>Kennyl</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Larry</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>zoe@gmail.com</t>
-  </si>
-  <si>
     <t>k@gmail.com</t>
   </si>
   <si>
@@ -61,6 +49,24 @@
   </si>
   <si>
     <t>Garry@gmail.com</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Glin</t>
+  </si>
+  <si>
+    <t>Mop</t>
+  </si>
+  <si>
+    <t>Drop</t>
   </si>
 </sst>
 </file>
@@ -427,68 +433,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{51A8B2B7-5845-444F-A154-DA113F7EB503}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{89ADF3AF-5AA9-6742-9968-8243525C4E2B}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{859321DA-A95F-B241-8B54-19957DE13C76}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{7C1F439D-AC4C-B349-9390-7D13038F7019}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{89ADF3AF-5AA9-6742-9968-8243525C4E2B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{859321DA-A95F-B241-8B54-19957DE13C76}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{7C1F439D-AC4C-B349-9390-7D13038F7019}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel reader not working
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D43ADBD-2478-154E-925B-7A76CFA64313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC91861-0AFA-514E-B83D-66CFC3683FE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Larry</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -42,15 +39,6 @@
     <t>k@gmail.com</t>
   </si>
   <si>
-    <t>larry@gmail.com</t>
-  </si>
-  <si>
-    <t>Garry</t>
-  </si>
-  <si>
-    <t>Garry@gmail.com</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -63,17 +51,36 @@
     <t>Glin</t>
   </si>
   <si>
-    <t>Mop</t>
-  </si>
-  <si>
-    <t>Drop</t>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Refcode</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>2021-04-23 14:49:41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,20 +114,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,67 +444,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{89ADF3AF-5AA9-6742-9968-8243525C4E2B}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{859321DA-A95F-B241-8B54-19957DE13C76}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{7C1F439D-AC4C-B349-9390-7D13038F7019}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
donor data used with uploads
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1ECB87-96CC-6545-8448-27C55508517A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E245989-8192-314D-B510-C90A5034BEDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -31,26 +31,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>k@gmail.com</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
     <t>LastName</t>
   </si>
   <si>
-    <t>Ken</t>
-  </si>
-  <si>
-    <t>Glin</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -63,9 +54,6 @@
     <t>First</t>
   </si>
   <si>
-    <t>2021-04-23 14:49:41</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -75,9 +63,6 @@
     <t>jd@gmail.com</t>
   </si>
   <si>
-    <t>2021-03-24 14:49:41</t>
-  </si>
-  <si>
     <t>kayb@gmail.com</t>
   </si>
   <si>
@@ -87,7 +72,10 @@
     <t>Coms</t>
   </si>
   <si>
-    <t>2021-05-12 14:49:41</t>
+    <t>2021-04-24 15:49:41</t>
+  </si>
+  <si>
+    <t>2021-04-12 11:49:41</t>
   </si>
 </sst>
 </file>
@@ -468,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,44 +477,44 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -535,40 +523,19 @@
         <v>12</v>
       </c>
       <c r="D3" s="5">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{89ADF3AF-5AA9-6742-9968-8243525C4E2B}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{7F620A17-A4BA-B74D-AC39-97B70F6C75F1}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{F0ED6F7F-CAEC-384F-A668-6A720C482079}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7F620A17-A4BA-B74D-AC39-97B70F6C75F1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F0ED6F7F-CAEC-384F-A668-6A720C482079}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
import emails added to controller
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E245989-8192-314D-B510-C90A5034BEDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82408F84-CC89-A747-8599-C556CD662FC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -72,10 +72,10 @@
     <t>Coms</t>
   </si>
   <si>
-    <t>2021-04-24 15:49:41</t>
-  </si>
-  <si>
-    <t>2021-04-12 11:49:41</t>
+    <t>2021-05-14 10:49:41</t>
+  </si>
+  <si>
+    <t>2021-05-24 17:39:41</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,10 +503,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -526,7 +526,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
user uploader working on emails
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B730DDC-5846-DF41-A89F-CAFF4ECE6110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDDCE97-A5DE-804F-BF03-AA12205122E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -31,20 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -54,45 +45,20 @@
     <t>First</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>jd@gmail.com</t>
-  </si>
-  <si>
-    <t>kayb@gmail.com</t>
-  </si>
-  <si>
-    <t>Kayla</t>
-  </si>
-  <si>
-    <t>Coms</t>
-  </si>
-  <si>
-    <t>2021-05-14 10:49:41</t>
-  </si>
-  <si>
     <t>2021-05-24 17:39:41</t>
+  </si>
+  <si>
+    <t>2021-04-24 17:39:41</t>
+  </si>
+  <si>
+    <t>Second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,24 +92,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,23 +419,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="18.6640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -482,60 +442,32 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{F0ED6F7F-CAEC-384F-A668-6A720C482079}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{7F620A17-A4BA-B74D-AC39-97B70F6C75F1}"/>
+    <hyperlink ref="A2" r:id="rId1" display="jd@gmail.com" xr:uid="{7F620A17-A4BA-B74D-AC39-97B70F6C75F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sorting working for emails with committees
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A22F4D-91F6-CC42-AF61-276CEC9BCF9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B24CB0F-7967-ED47-AC1F-A074B31C2CB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Refcode</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -72,10 +69,16 @@
     <t>Coms</t>
   </si>
   <si>
-    <t>2021-05-14 10:49:41</t>
-  </si>
-  <si>
-    <t>2021-05-24 17:39:41</t>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>2021-05-14 17:39:41</t>
+  </si>
+  <si>
+    <t>2021-05-24 10:49:41</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,13 +497,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="5">
         <v>5</v>
@@ -509,27 +512,27 @@
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="5">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel working with committees
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B24CB0F-7967-ED47-AC1F-A074B31C2CB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5204C1-0D25-FF4B-924E-EFF3B55FEA58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -51,6 +51,9 @@
     <t>Refcode</t>
   </si>
   <si>
+    <t>First</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
@@ -69,16 +72,13 @@
     <t>Coms</t>
   </si>
   <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>2021-05-14 17:39:41</t>
-  </si>
-  <si>
-    <t>2021-05-24 10:49:41</t>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>2021-05-25 10:49:41</t>
+  </si>
+  <si>
+    <t>2021-05-15 17:39:41</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,39 +497,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="5">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5">
-        <v>5</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
donations upload working with donations copy stop
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5204C1-0D25-FF4B-924E-EFF3B55FEA58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A519A190-4226-1942-8B05-7C267A3E9EFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
+    <workbookView xWindow="7640" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Amount</t>
   </si>
@@ -79,6 +70,39 @@
   </si>
   <si>
     <t>2021-05-15 17:39:41</t>
+  </si>
+  <si>
+    <t>Receipt ID</t>
+  </si>
+  <si>
+    <t>Recurring Total Months</t>
+  </si>
+  <si>
+    <t>Recurrence Number</t>
+  </si>
+  <si>
+    <t>AB122591002</t>
+  </si>
+  <si>
+    <t>2021-03-01 04:38:26</t>
+  </si>
+  <si>
+    <t>AB135987556</t>
+  </si>
+  <si>
+    <t>2021-03-01 04:44:51</t>
+  </si>
+  <si>
+    <t>unlimited</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -88,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +134,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,15 +172,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -459,80 +503,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="6" width="18.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="5">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6">
+        <v>12</v>
+      </c>
+      <c r="I2" s="6">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="5">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
donor info working on upload
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A519A190-4226-1942-8B05-7C267A3E9EFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A754D19-0A71-E940-956B-8AFEA32D6129}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t>larry@gmail.com</t>
+  </si>
+  <si>
+    <t>Garry</t>
+  </si>
+  <si>
+    <t>Garry@gmail.com</t>
+  </si>
+  <si>
+    <t>Mop</t>
+  </si>
+  <si>
+    <t>Drop</t>
+  </si>
   <si>
     <t>Amount</t>
   </si>
@@ -42,18 +66,6 @@
     <t>Refcode</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>jd@gmail.com</t>
-  </si>
-  <si>
     <t>kayb@gmail.com</t>
   </si>
   <si>
@@ -63,13 +75,7 @@
     <t>Coms</t>
   </si>
   <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>2021-05-25 10:49:41</t>
-  </si>
-  <si>
-    <t>2021-05-15 17:39:41</t>
+    <t>Fourth</t>
   </si>
   <si>
     <t>Receipt ID</t>
@@ -96,30 +102,80 @@
     <t>unlimited</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+    <t>Donor First Name</t>
+  </si>
+  <si>
+    <t>Donor Last Name</t>
+  </si>
+  <si>
+    <t>Donor Addr1</t>
+  </si>
+  <si>
+    <t>Donor City</t>
+  </si>
+  <si>
+    <t>Donor State</t>
+  </si>
+  <si>
+    <t>Donor ZIP</t>
+  </si>
+  <si>
+    <t>Donor Country</t>
+  </si>
+  <si>
+    <t>Donor Email</t>
+  </si>
+  <si>
+    <t>Donor Phone</t>
+  </si>
+  <si>
+    <t>9899 warrick trail dr. 433</t>
+  </si>
+  <si>
+    <t>newburgh</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>251 Indian hills drive</t>
+  </si>
+  <si>
+    <t>Corydon</t>
+  </si>
+  <si>
+    <t>AB192115731</t>
+  </si>
+  <si>
+    <t>2021-03-01 09:00:30</t>
+  </si>
+  <si>
+    <t>2120 S Salem Rd</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>AB192116789</t>
+  </si>
+  <si>
+    <t>2021-03-01 09:34:58</t>
+  </si>
+  <si>
+    <t>zoemking63@gmail.com</t>
+  </si>
+  <si>
+    <t>King</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,16 +192,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -167,30 +215,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,122 +549,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="6" width="18.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="18.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3">
+        <v>47630</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2173412144</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E3" s="3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="3">
+        <v>47112</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="3">
+        <v>46772</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2602235736</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="3">
+        <v>46772</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="6">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="6">
-        <v>8</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>10</v>
+      <c r="N5" s="3">
+        <v>2602235736</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7F620A17-A4BA-B74D-AC39-97B70F6C75F1}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F0ED6F7F-CAEC-384F-A668-6A720C482079}"/>
+    <hyperlink ref="M4" r:id="rId1" xr:uid="{B92BEB40-089C-F44D-B6D7-97B3E2CD6AD2}"/>
+    <hyperlink ref="M5" r:id="rId2" xr:uid="{523035A4-8F35-5D4D-AFD0-26CF2929043A}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{25659A0C-EF45-504B-A225-129AF87AD39C}"/>
+    <hyperlink ref="M3" r:id="rId4" xr:uid="{F588222F-412E-594F-9FF5-1D6030C13526}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new email on donatiation working
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A754D19-0A71-E940-956B-8AFEA32D6129}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988A7929-E28E-7947-8197-88F4F34BB023}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -34,28 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Larry</t>
-  </si>
-  <si>
-    <t>larry@gmail.com</t>
-  </si>
-  <si>
-    <t>Garry</t>
-  </si>
-  <si>
-    <t>Garry@gmail.com</t>
-  </si>
-  <si>
-    <t>Mop</t>
-  </si>
-  <si>
-    <t>Drop</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Amount</t>
   </si>
@@ -63,21 +42,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Refcode</t>
-  </si>
-  <si>
-    <t>kayb@gmail.com</t>
-  </si>
-  <si>
-    <t>Kayla</t>
-  </si>
-  <si>
-    <t>Coms</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
     <t>Receipt ID</t>
   </si>
   <si>
@@ -87,21 +51,6 @@
     <t>Recurrence Number</t>
   </si>
   <si>
-    <t>AB122591002</t>
-  </si>
-  <si>
-    <t>2021-03-01 04:38:26</t>
-  </si>
-  <si>
-    <t>AB135987556</t>
-  </si>
-  <si>
-    <t>2021-03-01 04:44:51</t>
-  </si>
-  <si>
-    <t>unlimited</t>
-  </si>
-  <si>
     <t>Donor First Name</t>
   </si>
   <si>
@@ -141,34 +90,25 @@
     <t>United States</t>
   </si>
   <si>
-    <t>251 Indian hills drive</t>
-  </si>
-  <si>
-    <t>Corydon</t>
-  </si>
-  <si>
-    <t>AB192115731</t>
-  </si>
-  <si>
-    <t>2021-03-01 09:00:30</t>
-  </si>
-  <si>
-    <t>2120 S Salem Rd</t>
-  </si>
-  <si>
-    <t>Monroe</t>
-  </si>
-  <si>
-    <t>AB192116789</t>
-  </si>
-  <si>
-    <t>2021-03-01 09:34:58</t>
-  </si>
-  <si>
-    <t>zoemking63@gmail.com</t>
-  </si>
-  <si>
-    <t>King</t>
+    <t>Reference code</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Dons</t>
+  </si>
+  <si>
+    <t>donnab@gmail.com</t>
+  </si>
+  <si>
+    <t>2021-05-24 04:48:26</t>
+  </si>
+  <si>
+    <t>tester3</t>
+  </si>
+  <si>
+    <t>AB522571038</t>
   </si>
 </sst>
 </file>
@@ -549,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4CA718-8E57-CC4B-9644-44692EDFB230}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,57 +507,57 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>10</v>
@@ -629,179 +569,39 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="K2" s="3">
         <v>47630</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="N2" s="3">
         <v>2173412144</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="3">
-        <v>47112</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="3">
-        <v>46772</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="3">
-        <v>2602235736</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="3">
-        <v>46772</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="3">
-        <v>2602235736</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M4" r:id="rId1" xr:uid="{B92BEB40-089C-F44D-B6D7-97B3E2CD6AD2}"/>
-    <hyperlink ref="M5" r:id="rId2" xr:uid="{523035A4-8F35-5D4D-AFD0-26CF2929043A}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{25659A0C-EF45-504B-A225-129AF87AD39C}"/>
-    <hyperlink ref="M3" r:id="rId4" xr:uid="{F588222F-412E-594F-9FF5-1D6030C13526}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{25659A0C-EF45-504B-A225-129AF87AD39C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create email from donation is not getting email data
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988A7929-E28E-7947-8197-88F4F34BB023}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF644FF-2D29-3F4D-8ACC-E9C9E7CE4860}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -105,10 +105,10 @@
     <t>2021-05-24 04:48:26</t>
   </si>
   <si>
-    <t>tester3</t>
-  </si>
-  <si>
-    <t>AB522571038</t>
+    <t>AB522581037</t>
+  </si>
+  <si>
+    <t>tester11</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -596,7 +596,7 @@
         <v>2173412144</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create email from donation with email data is not working
</commit_message>
<xml_diff>
--- a/D:\test excel\Test.xlsx
+++ b/D:\test excel\Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF644FF-2D29-3F4D-8ACC-E9C9E7CE4860}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7BF3F9-B66B-4A49-84C2-B7F484014514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{367EC722-CC7E-6C4B-AF0F-8BE1CD29E107}"/>
   </bookViews>
@@ -105,10 +105,10 @@
     <t>2021-05-24 04:48:26</t>
   </si>
   <si>
-    <t>AB522581037</t>
-  </si>
-  <si>
-    <t>tester11</t>
+    <t>tester16</t>
+  </si>
+  <si>
+    <t>AB522581043</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -596,7 +596,7 @@
         <v>2173412144</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>